<commit_message>
Modified R33 resistor value which caused gain error, for transimpedance amplifier in first prototypes of V0.2 design.
</commit_message>
<xml_diff>
--- a/hardware/pcbs/teensy_shield_v0p2/BOM_FULL.xlsx
+++ b/hardware/pcbs/teensy_shield_v0p2/BOM_FULL.xlsx
@@ -170,7 +170,7 @@
     <t xml:space="preserve">12k Resistor,  1%</t>
   </si>
   <si>
-    <t xml:space="preserve">R1,R2,R26,R28,R34,R36</t>
+    <t xml:space="preserve">R1,R2,R26,R28,R34,R36,R33</t>
   </si>
   <si>
     <t xml:space="preserve">C22790 </t>
@@ -179,7 +179,7 @@
     <t xml:space="preserve">20k Resistor, 1%</t>
   </si>
   <si>
-    <t xml:space="preserve">R3,R5,R6,R8,R10,R13,R23,R25,R29,R33</t>
+    <t xml:space="preserve">R3,R5,R6,R8,R10,R13,R23,R25,R29</t>
   </si>
   <si>
     <t xml:space="preserve">C4184 </t>
@@ -703,13 +703,13 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="66.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.78"/>

</xml_diff>

<commit_message>
Fixed quantities in BOM after component change.
</commit_message>
<xml_diff>
--- a/hardware/pcbs/teensy_shield_v0p2/BOM_FULL.xlsx
+++ b/hardware/pcbs/teensy_shield_v0p2/BOM_FULL.xlsx
@@ -703,13 +703,13 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="66.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.78"/>
@@ -916,7 +916,7 @@
         <v>36</v>
       </c>
       <c r="E13" s="9" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -933,7 +933,7 @@
         <v>39</v>
       </c>
       <c r="E14" s="9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>